<commit_message>
minor changes on the profile
</commit_message>
<xml_diff>
--- a/docs/profiles/StructureDefinition-mhero-comm-req-broadcast-starts.xlsx
+++ b/docs/profiles/StructureDefinition-mhero-comm-req-broadcast-starts.xlsx
@@ -1894,7 +1894,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>44</v>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>44</v>

</xml_diff>